<commit_message>
Better understanding of the data we are manipulating
</commit_message>
<xml_diff>
--- a/chapter 2/my_data_with_signals.xlsx
+++ b/chapter 2/my_data_with_signals.xlsx
@@ -941,7 +941,7 @@
         <v>1.235299944877625</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1757,7 +1757,7 @@
         <v>1.227385401725769</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2386,7 +2386,7 @@
         <v>1.17475688457489</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2675,7 +2675,7 @@
         <v>1.169385552406311</v>
       </c>
       <c r="E135">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -4375,7 +4375,7 @@
         <v>1.140263795852661</v>
       </c>
       <c r="E235">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="236" spans="1:5">
@@ -4596,7 +4596,7 @@
         <v>1.132284879684448</v>
       </c>
       <c r="E248">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="249" spans="1:5">
@@ -4681,7 +4681,7 @@
         <v>1.137565851211548</v>
       </c>
       <c r="E253">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="254" spans="1:5">
@@ -5599,7 +5599,7 @@
         <v>1.133825421333313</v>
       </c>
       <c r="E307">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="308" spans="1:5">
@@ -5718,7 +5718,7 @@
         <v>1.133285760879517</v>
       </c>
       <c r="E314">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="315" spans="1:5">
@@ -6160,7 +6160,7 @@
         <v>1.123608112335205</v>
       </c>
       <c r="E340">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="341" spans="1:5">
@@ -6483,7 +6483,7 @@
         <v>1.12095057964325</v>
       </c>
       <c r="E359">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="360" spans="1:5">
@@ -7520,7 +7520,7 @@
         <v>1.120686769485474</v>
       </c>
       <c r="E420">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="421" spans="1:5">
@@ -8268,7 +8268,7 @@
         <v>1.101442933082581</v>
       </c>
       <c r="E464">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="465" spans="1:5">
@@ -8897,7 +8897,7 @@
         <v>1.107603788375854</v>
       </c>
       <c r="E501">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="502" spans="1:5">
@@ -11413,7 +11413,7 @@
         <v>1.122082591056824</v>
       </c>
       <c r="E649">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="650" spans="1:5">
@@ -11481,7 +11481,7 @@
         <v>1.125340342521667</v>
       </c>
       <c r="E653">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="654" spans="1:5">
@@ -12705,7 +12705,7 @@
         <v>1.181334972381592</v>
       </c>
       <c r="E725">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="726" spans="1:5">
@@ -13198,7 +13198,7 @@
         <v>1.18674647808075</v>
       </c>
       <c r="E754">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="755" spans="1:5">
@@ -14320,7 +14320,7 @@
         <v>1.212444543838501</v>
       </c>
       <c r="E820">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="821" spans="1:5">
@@ -15578,7 +15578,7 @@
         <v>1.213029861450195</v>
       </c>
       <c r="E894">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="895" spans="1:5">
@@ -16853,7 +16853,7 @@
         <v>1.17648446559906</v>
       </c>
       <c r="E969">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="970" spans="1:5">
@@ -17924,7 +17924,7 @@
         <v>1.125872611999512</v>
       </c>
       <c r="E1032">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1033" spans="1:5">
@@ -18111,7 +18111,7 @@
         <v>1.135976433753967</v>
       </c>
       <c r="E1043">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1044" spans="1:5">
@@ -19199,7 +19199,7 @@
         <v>1.109151601791382</v>
       </c>
       <c r="E1107">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1108" spans="1:5">
@@ -19267,7 +19267,7 @@
         <v>1.097586393356323</v>
       </c>
       <c r="E1111">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1112" spans="1:5">
@@ -20746,7 +20746,7 @@
         <v>1.015764594078064</v>
       </c>
       <c r="E1198">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1199" spans="1:5">
@@ -20797,7 +20797,7 @@
         <v>1.019762992858887</v>
       </c>
       <c r="E1201">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="1202" spans="1:5">
@@ -22599,7 +22599,7 @@
         <v>1.054685473442078</v>
       </c>
       <c r="E1307">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="1308" spans="1:5">
@@ -23415,7 +23415,7 @@
         <v>1.06836462020874</v>
       </c>
       <c r="E1355">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1356" spans="1:5">
@@ -23483,7 +23483,7 @@
         <v>1.061413407325745</v>
       </c>
       <c r="E1359">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1360" spans="1:5">
@@ -24826,7 +24826,7 @@
         <v>1.085658431053162</v>
       </c>
       <c r="E1438">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="1439" spans="1:5">
@@ -25166,7 +25166,7 @@
         <v>1.094415187835693</v>
       </c>
       <c r="E1458">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="1459" spans="1:5">
@@ -27087,7 +27087,7 @@
         <v>1.095170259475708</v>
       </c>
       <c r="E1571">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="1572" spans="1:5">
@@ -27750,7 +27750,7 @@
         <v>1.084269404411316</v>
       </c>
       <c r="E1610">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1611" spans="1:5">
@@ -28583,7 +28583,7 @@
         <v>1.078515887260437</v>
       </c>
       <c r="E1659">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1660" spans="1:5">
@@ -29552,7 +29552,7 @@
         <v>1.081946611404419</v>
       </c>
       <c r="E1716">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="1717" spans="1:5">
@@ -30062,7 +30062,7 @@
         <v>1.103752732276917</v>
       </c>
       <c r="E1746">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="1747" spans="1:5">
@@ -30249,7 +30249,7 @@
         <v>1.119119048118591</v>
       </c>
       <c r="E1757">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1758" spans="1:5">
@@ -31133,7 +31133,7 @@
         <v>1.058559536933899</v>
       </c>
       <c r="E1809">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1810" spans="1:5">
@@ -31201,7 +31201,7 @@
         <v>1.050685048103333</v>
       </c>
       <c r="E1813">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1814" spans="1:5">
@@ -31898,7 +31898,7 @@
         <v>1.031161665916443</v>
       </c>
       <c r="E1854">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="1855" spans="1:5">
@@ -32510,7 +32510,7 @@
         <v>1.08188807964325</v>
       </c>
       <c r="E1890">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="1891" spans="1:5">
@@ -33207,7 +33207,7 @@
         <v>1.137837648391724</v>
       </c>
       <c r="E1931">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1932" spans="1:5">
@@ -33836,7 +33836,7 @@
         <v>1.169453859329224</v>
       </c>
       <c r="E1968">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="1969" spans="1:5">
@@ -34244,7 +34244,7 @@
         <v>1.170960187911987</v>
       </c>
       <c r="E1992">
-        <v>0</v>
+        <v>7777</v>
       </c>
     </row>
     <row r="1993" spans="1:5">
@@ -34295,7 +34295,7 @@
         <v>1.164795279502869</v>
       </c>
       <c r="E1995">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="1996" spans="1:5">
@@ -34652,7 +34652,7 @@
         <v>1.166275978088379</v>
       </c>
       <c r="E2016">
-        <v>0</v>
+        <v>8888</v>
       </c>
     </row>
     <row r="2017" spans="1:5">

</xml_diff>